<commit_message>
Hoàn Thành phần tạo pan vs Tổng hợp (còn thiếu hình1 ) 29.12.2023
</commit_message>
<xml_diff>
--- a/Đo_An/HoanThanhDangNhap/bin/Debug/Resources/Du lieu cau hoi/thu vien ma loi.xlsx
+++ b/Đo_An/HoanThanhDangNhap/bin/Debug/Resources/Du lieu cau hoi/thu vien ma loi.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Đăng_Quý_UTE_K19\Đo_An\HoanThanhDangNhap\bin\Debug\Resources\Du lieu cau hoi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\OneDrive\Desktop\Resources\Du lieu cau hoi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA3BB25-25AD-420A-B6FE-EA3F269BA03E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="13" xr2:uid="{59E887D8-2F98-4F00-A936-BD1BC32CA0BD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="15" r:id="rId1"/>
@@ -26,9 +25,8 @@
     <sheet name="11" sheetId="3" r:id="rId11"/>
     <sheet name="12" sheetId="4" r:id="rId12"/>
     <sheet name="13" sheetId="5" r:id="rId13"/>
-    <sheet name="14" sheetId="6" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="116">
   <si>
     <t>dap an 2</t>
   </si>
@@ -73,9 +71,6 @@
     <t>Hiện tượng</t>
   </si>
   <si>
-    <t>Hiện tượng a</t>
-  </si>
-  <si>
     <t>Ki tu loi</t>
   </si>
   <si>
@@ -91,42 +86,15 @@
     <t>13</t>
   </si>
   <si>
-    <t>HINH</t>
-  </si>
-  <si>
     <t>COMP</t>
   </si>
   <si>
-    <t>\\Resources\\mach c6.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Comp1, Comp2, Comp3, Comp4</t>
-  </si>
-  <si>
-    <t>\\Resources\\mach trang.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Comp3, Comp5, Comp7, Comp10</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CB (#1), Công tắc mở cốp (#2), Cuộn dây relay (#9), GND</t>
-  </si>
-  <si>
     <t>11</t>
   </si>
   <si>
     <t>15</t>
   </si>
   <si>
-    <t>Hở mass</t>
-  </si>
-  <si>
-    <t>Mass có thêm điện trở</t>
-  </si>
-  <si>
-    <t>Công tắc số 2 bị hở</t>
-  </si>
-  <si>
     <t>\\Resources\\tong hop final wiring\\c5.png</t>
   </si>
   <si>
@@ -136,9 +104,6 @@
     <t>05</t>
   </si>
   <si>
-    <t xml:space="preserve"> CB (#1), Relay còi (#9), Còi (#11), Công tắc còi (#17), GND</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
@@ -151,9 +116,6 @@
     <t>06</t>
   </si>
   <si>
-    <t xml:space="preserve"> CB (#1), Công tắc đèn lùi (#10), Đèn #12, Đèn #15, GND</t>
-  </si>
-  <si>
     <t>6</t>
   </si>
   <si>
@@ -166,48 +128,21 @@
     <t>20</t>
   </si>
   <si>
-    <t xml:space="preserve"> CB (#1), Công tắc đèn phanh (#2), Công tắc đèn đầu (#8), Đèn phanh trái (#12), Đèn đuôi trái (#13), Đèn phanh phải (#14), Đèn đuôi phải (#15), GND</t>
-  </si>
-  <si>
     <t>17</t>
   </si>
   <si>
-    <t xml:space="preserve"> Cầu chì ngắt mạch (#1), Điện trở #3, Điện trở #4, Điện trở #7, GND</t>
-  </si>
-  <si>
     <t>\\Resources\\tong hop final wiring\\c1.png</t>
   </si>
   <si>
     <t>\\Resources\\tong hop final wiring\\c2.png</t>
   </si>
   <si>
-    <t xml:space="preserve"> Cầu chì ngắt mạch (#1), Điện trở #3, Điện trở #4, Điện trở #5, Điện trở #7, GND </t>
-  </si>
-  <si>
     <t>\\Resources\\tong hop final wiring\\c3.png</t>
   </si>
   <si>
-    <t xml:space="preserve"> Cầu chì ngắt mạch (#1), Relay còi(#9), Còi (#11), Công tắc còi (#17), GND</t>
-  </si>
-  <si>
     <t>\\Resources\\tong hop final wiring\\c4.png</t>
   </si>
   <si>
-    <t xml:space="preserve"> Cầu chì ngắt mạch (#1), Công tắc đèn lùi (#10), Đèn #12, Đèn #15, GND</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cầu chì ngắt mạch (#1), Công tắc đèn phanh (#2), Công tắc đèn đầu (#8), Đèn phanh trái (#12), Đèn đuôi trái (#13), Đèn đuôi phải (#14), Đèn phanh phải (#15), GND</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cầu chì ngắt mạch (#1), Công tắc P/N (#8), Relay máy đề (#9), Công tắc đánh lửa (#10), Motor máy đề (#16), GND</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cầu chì ngắt mạch (#1), Bộ chớp (flasher) (#2), Công tắc xi nhan (#8), Công tắc đèn báo đỗ (#10), Đèn đỗ (#12), Đèn báo bên hông (#13), Đèn báo rẽ (#14), Đèn xinhan (#15), GND</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cầu chì ngắt mạch (#1), Công tắc đèn (#8), Công tắc đèn mờ (#10), Đèn pha trái (#12), Đèn cốt trái (#13), Đèn cốt phải (#14), Đèn pha phải (#15), GND</t>
-  </si>
-  <si>
     <t>p1</t>
   </si>
   <si>
@@ -281,13 +216,266 @@
   </si>
   <si>
     <t>p16</t>
+  </si>
+  <si>
+    <t>Hình 2</t>
+  </si>
+  <si>
+    <t>Hình 1</t>
+  </si>
+  <si>
+    <t>Yêu cầu 1</t>
+  </si>
+  <si>
+    <t>Yêu cầu 2</t>
+  </si>
+  <si>
+    <t>Sinh viên kết nối thiết bị như hình bên</t>
+  </si>
+  <si>
+    <t>Hướng dẫn: 
+Thực hành đo kiểm trên vùng được đánh dấu ở hình bên tìm lỗi hệ thống và chọn đáp án.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sinh viên </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>sử dụng bộ đo gió van trượt và bơm nhiên liệu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, kết nối thiết bị như hình bên</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sinh viên </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>sử dụng Delco Hall và bơm nhiên liệu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, kết nối thiết bị như hình bên</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sinh viên </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>sử dụng Bô bin đánh lửa trực tiếp CÓ tích hợp Transistor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, kết nối thiết bị như hình bên</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sinh viên </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>sử dụng Kim phun loại điện trở cao</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, kết nối thiết bị như hình bên</t>
+    </r>
+  </si>
+  <si>
+    <t>\\Resources\\tong hop final wiring\\2.png</t>
+  </si>
+  <si>
+    <t>\\Resources\\tong hop final wiring\\4.png</t>
+  </si>
+  <si>
+    <t>\\Resources\\tong hop final wiring\\6.png</t>
+  </si>
+  <si>
+    <t>\\Resources\\tong hop final wiring\\8.png</t>
+  </si>
+  <si>
+    <t>\\Resources\\tong hop final wiring\\10.png</t>
+  </si>
+  <si>
+    <t>\\Resources\\tong hop final wiring\\12.png</t>
+  </si>
+  <si>
+    <t>\\Resources\\tong hop final wiring\\14.png</t>
+  </si>
+  <si>
+    <t>\\Resources\\tong hop final wiring\\16.png</t>
+  </si>
+  <si>
+    <t>\\Resources\\tong hop final wiring\\18.png</t>
+  </si>
+  <si>
+    <t>\\Resources\\tong hop final wiring\\20.png</t>
+  </si>
+  <si>
+    <t>\\Resources\\tong hop final wiring\\22.png</t>
+  </si>
+  <si>
+    <t>\\Resources\\tong hop final wiring\\24.png</t>
+  </si>
+  <si>
+    <t>\\Resources\\tong hop final wiring\\26.png</t>
+  </si>
+  <si>
+    <t>\\Resources\\tong hop final wiring\\30.png</t>
+  </si>
+  <si>
+    <t>\\Resources\\tong hop final wiring\\28.png</t>
+  </si>
+  <si>
+    <t>\\Resources\\tong hop final wiring\\32.png</t>
+  </si>
+  <si>
+    <t>\\Resources\\tong hop final wiring\\34.png</t>
+  </si>
+  <si>
+    <t>\\Resources\\tong hop final wiring\\36.png</t>
+  </si>
+  <si>
+    <t>Ngắn mạch VC</t>
+  </si>
+  <si>
+    <t>Trở đường dây</t>
+  </si>
+  <si>
+    <t>Ngắn mạch</t>
+  </si>
+  <si>
+    <t>Ngắn mạch GND</t>
+  </si>
+  <si>
+    <t>p20</t>
+  </si>
+  <si>
+    <t>COMP2</t>
+  </si>
+  <si>
+    <t>Ngắn mạch B+</t>
+  </si>
+  <si>
+    <t>Đường dây E2,Đường dây +B,Đường dây VG,Đường dây THA,Đường dây EVG</t>
+  </si>
+  <si>
+    <t>Hở mạch,Ngắn mạch GND,Ngắn mạch nguồn,Điện trở không mong muốn</t>
+  </si>
+  <si>
+    <t>Đường dây E2,Đường dây +B,Đường dây KS,Đường dây THA,Đường dây PA</t>
+  </si>
+  <si>
+    <t>Hở mạch,Ngắn mạch GND,Ngắn mạch nguồn 12V,Ngắn mạch VC,Điện trở không mong muốn</t>
+  </si>
+  <si>
+    <t>Đường dây E2,Đường dây VC,Đường dây VS,Đường dây THA,Đường dây FC</t>
+  </si>
+  <si>
+    <t>Hở mạch,Ngắn mạch,Ngắn mạch VC,Điện trở không mong muốn</t>
+  </si>
+  <si>
+    <t>Đường dây E2,Đường dây VC,Đường dây PIM</t>
+  </si>
+  <si>
+    <t>Hở mạch,Ngắn mạch GND,Ngắn mạch VC,Điện trở không mong muốn</t>
+  </si>
+  <si>
+    <t>Hở mạch,Ngắn mạch,Ngắn mạch VC, Điện trở không mong muốn</t>
+  </si>
+  <si>
+    <t>Đường dây +B,Đường dây NE+,Đường dây E2</t>
+  </si>
+  <si>
+    <t>Đường dây E2,Đường dây TH</t>
+  </si>
+  <si>
+    <t>Hở mạch,Ngắn mạch GND,Điện trở không mong muốn</t>
+  </si>
+  <si>
+    <t>Đường dây PSW,Đường dây E2,Đường dây IDL</t>
+  </si>
+  <si>
+    <t>Đường dây VC,Đường dây VTA,Đường dây IDL,Đường dây E2</t>
+  </si>
+  <si>
+    <t>Hở mạch,Ngắn mạch VC,Ngắn mạch GND,Điện trở không mong muốn</t>
+  </si>
+  <si>
+    <t>Đường dây VC,Đường dây VTA,Đường dây E2</t>
+  </si>
+  <si>
+    <t>Đường dây FC,Đường dây FP,Đường dây +B,Đường dây GND,Đường dây STA,Đường IG</t>
+  </si>
+  <si>
+    <t>Hở mạch,Ngắn mạch nguồn,Ngắn mạch GND,Điện trở không mong muốn</t>
+  </si>
+  <si>
+    <t>Đường dây GND,Đường dây #10,Đường +B</t>
+  </si>
+  <si>
+    <t>Đường dây GND,Đường dây IGT,Đường dây +B</t>
+  </si>
+  <si>
+    <t>Đường dây VC hoặc VCPA; VCPA2,Đường dây E2 hoặc EPA; EPA2,Đường dây VPA,Đường dây VPA2,Đường dây VPA và VPA2,Đường dây VTA,Đường dây VTA2,Đường dây VTA và VTA2,Đường dây M+,Đường dây M-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -336,6 +524,19 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -351,7 +552,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -394,10 +595,21 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -405,7 +617,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -415,11 +627,9 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -430,7 +640,36 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -745,21 +984,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1D49EAE-ED46-4B41-B154-AB332AE7AD2C}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="18.77734375" style="5"/>
     <col min="4" max="4" width="41.33203125" style="5" customWidth="1"/>
-    <col min="5" max="16384" width="18.77734375" style="5"/>
+    <col min="5" max="5" width="18.77734375" style="5"/>
+    <col min="6" max="6" width="46.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.77734375" style="5"/>
+    <col min="8" max="8" width="194.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="66.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="18.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -773,39 +1017,63 @@
         <v>10</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="101.4" x14ac:dyDescent="0.35">
+      <c r="A2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="D2" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="101.4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -815,42 +1083,281 @@
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>27</v>
+      <c r="D3" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" s="15" t="s">
         <v>44</v>
       </c>
+      <c r="F3" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="K3" s="29" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+    </row>
+    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+    </row>
+    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+    </row>
+    <row r="7" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+    </row>
+    <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+    </row>
+    <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+    </row>
+    <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A10" s="19"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+    </row>
+    <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+    </row>
+    <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+    </row>
+    <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+    </row>
+    <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+    </row>
+    <row r="15" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+    </row>
+    <row r="16" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+    </row>
+    <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+    </row>
+    <row r="18" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+    </row>
+    <row r="19" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+    </row>
+    <row r="20" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+    </row>
+    <row r="21" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{26546DD6-55E8-414A-9DFF-E032C98F878E}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{08512137-2C17-49FB-823F-C1BAB963CBDC}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="G2" r:id="rId3"/>
+    <hyperlink ref="G3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E6CA380-593F-4D6D-BD19-E23722A1ACB3}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="14.21875" style="5"/>
+    <col min="1" max="7" width="14.21875" style="5"/>
+    <col min="8" max="8" width="41.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.5546875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="31.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="14.21875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -864,63 +1371,167 @@
         <v>10</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="115.8" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="I2" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="180" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="7" t="s">
+      <c r="B3" s="2" t="s">
         <v>22</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="I3" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K3" s="31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="180" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="I4" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K4" s="31" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00401BD7-D03E-4289-8CE4-8DA0E14241CB}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId2"/>
+    <hyperlink ref="F3" r:id="rId3"/>
+    <hyperlink ref="F4" r:id="rId4"/>
+    <hyperlink ref="G3" r:id="rId5"/>
+    <hyperlink ref="G4" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2C51666-D7EB-48DB-B030-4AF6B6FAC783}">
-  <dimension ref="A1:G17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.6640625" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="3" width="19.6640625" style="1"/>
     <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="19.6640625" style="1"/>
+    <col min="5" max="7" width="19.6640625" style="1"/>
+    <col min="8" max="8" width="84.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="84.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="96.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="19.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -934,138 +1545,153 @@
         <v>10</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="126" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>26</v>
+      <c r="D2" s="11" t="s">
+        <v>91</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G9" s="12"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G10" s="12"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G11" s="12"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G12" s="12"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G13" s="12"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G14" s="12"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G15" s="12"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G16" s="12"/>
-    </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G17" s="12"/>
+        <v>46</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="I2" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" s="31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="33"/>
+      <c r="K3" s="31"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="33"/>
+      <c r="K4" s="31"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+    </row>
+    <row r="17" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{58B43EA4-C149-4FC8-B0EB-FB08ED441CE2}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{9DD0ED2E-6B97-46D0-9D28-746CC6851D5B}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{B7839C18-6FF0-4CF6-A575-C3C125E2115B}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{321D55E7-382B-4F67-BCC5-632BA812134C}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.6640625" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="3" width="15.6640625" style="1"/>
     <col min="4" max="4" width="30.88671875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="15.6640625" style="1"/>
+    <col min="5" max="7" width="15.6640625" style="1"/>
+    <col min="8" max="8" width="43.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43.5546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="108.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.88671875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="15.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1079,62 +1705,92 @@
         <v>10</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="108" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>26</v>
+        <v>6</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>32</v>
+        <v>49</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="I2" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="31" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{87587B73-32D2-4563-8098-2B3ABE58B0AF}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C75F4D7-2471-474B-ABB7-804021B454ED}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="3" width="13.6640625" style="1"/>
     <col min="4" max="4" width="40.44140625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="13.6640625" style="1"/>
+    <col min="5" max="7" width="13.6640625" style="1"/>
+    <col min="8" max="8" width="42.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42.5546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="83.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="38.6640625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="13.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1148,176 +1804,127 @@
         <v>10</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="90" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" s="31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="90" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>37</v>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K3" s="31" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{CF8EE311-9148-455B-B26B-678B33CC8C79}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B77FCA5-8F64-4A8B-9873-0423631D4835}">
-  <dimension ref="A1:G10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="3" width="13.6640625" style="1"/>
-    <col min="4" max="4" width="40.44140625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="13.6640625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="15"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="15"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="15"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="15"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="15"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="15"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="15"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{78EC6B83-3EE0-42C2-9E74-9FE30CCE5EF2}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{265D2BFE-E28B-4AAE-BBE1-1E23D79E99AD}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId2"/>
+    <hyperlink ref="F3" r:id="rId3"/>
+    <hyperlink ref="G3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0880F22E-F648-477F-AFB2-D3F86BE3DB51}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="16.21875" style="5"/>
     <col min="4" max="4" width="32.5546875" style="5" customWidth="1"/>
-    <col min="5" max="16384" width="16.21875" style="5"/>
+    <col min="5" max="7" width="16.21875" style="5"/>
+    <col min="8" max="8" width="68.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="68.6640625" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="16.21875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1331,16 +1938,28 @@
         <v>10</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="115.8" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1350,43 +1969,59 @@
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>26</v>
+      <c r="D2" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="I2" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>47</v>
+      <c r="K2" s="29" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{62129EA4-62C1-4111-A5DF-5887F3C735C2}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F1616E-2E6E-442F-9059-C2D807A1E0BD}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="16.77734375" style="5"/>
     <col min="4" max="4" width="44.21875" style="5" customWidth="1"/>
-    <col min="5" max="16384" width="16.77734375" style="5"/>
+    <col min="5" max="7" width="16.77734375" style="5"/>
+    <col min="8" max="8" width="68.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="68.6640625" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="16.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1400,41 +2035,65 @@
         <v>10</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="115.8" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>26</v>
+      <c r="D2" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:11" ht="115.8" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
@@ -1442,42 +2101,61 @@
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>27</v>
+      <c r="D3" s="14" t="s">
+        <v>88</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="K3" s="29" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{964037B5-1CDF-4FF4-97FD-7C6640E59EC8}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{30E56244-3198-4964-B99C-2A2BECBF72E8}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="G2" r:id="rId3"/>
+    <hyperlink ref="G3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3A416F-C220-415A-9CC2-56287BD2977C}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="45" customWidth="1"/>
+    <col min="6" max="6" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.21875" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1491,18 +2169,30 @@
         <v>10</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="101.4" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
@@ -1510,43 +2200,59 @@
       <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>26</v>
+      <c r="D2" s="14" t="s">
+        <v>89</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>51</v>
+        <v>48</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="J2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" s="30" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{240038C4-80DB-4243-B5F8-B8B403E559CE}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A19B6D-3F95-4600-9345-6B2A4BF2F2CD}">
-  <dimension ref="A1:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="42.5546875" customWidth="1"/>
     <col min="6" max="6" width="36.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="139.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.5546875" customWidth="1"/>
+    <col min="8" max="8" width="41.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.109375" customWidth="1"/>
+    <col min="10" max="10" width="31.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1560,18 +2266,30 @@
         <v>10</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="101.4" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -1579,65 +2297,80 @@
       <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>57</v>
+      <c r="D2" s="14" t="s">
+        <v>89</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="15"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="15"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
+        <v>50</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="J2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" s="30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="13"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="13"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="13"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="13"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="13"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="13"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="13"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{5DEAB3B8-3225-43C4-B6DD-9D08B5E938E0}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A64C6E32-9254-41AA-B630-CCA9A7D1DAE1}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="47.6640625" customWidth="1"/>
+    <col min="8" max="8" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1651,84 +2384,164 @@
         <v>10</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="115.8" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>26</v>
+      <c r="D2" s="14" t="s">
+        <v>90</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="J2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" s="30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="115.8" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>27</v>
+      <c r="D3" s="14" t="s">
+        <v>89</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="J3" t="s">
+        <v>64</v>
+      </c>
+      <c r="K3" s="30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="115.8" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="J4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K4" s="30" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{EDD8AA6B-F1DD-4DAD-BEED-FA42AD247800}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{6C52BB0F-F69A-4E0B-B482-CFC236794D44}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="G2" r:id="rId3"/>
+    <hyperlink ref="G3" r:id="rId4"/>
+    <hyperlink ref="F4" r:id="rId5"/>
+    <hyperlink ref="G4" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{936386D0-31DF-42AB-9347-C8052EEF6FC3}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="43.77734375" customWidth="1"/>
+    <col min="6" max="6" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.44140625" customWidth="1"/>
+    <col min="10" max="10" width="31.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1742,60 +2555,88 @@
         <v>10</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="115.8" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>26</v>
+        <v>8</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>89</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="J2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" s="30" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{94CE04F2-9D7E-4C5F-959E-2031CA53044D}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDE916D-7967-4764-B09B-7B94E16228BA}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="38.109375" customWidth="1"/>
+    <col min="8" max="8" width="42.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42.5546875" customWidth="1"/>
+    <col min="10" max="10" width="31.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1809,18 +2650,30 @@
         <v>10</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="130.19999999999999" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
@@ -1828,39 +2681,58 @@
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="16"/>
+      <c r="D2" s="14" t="s">
+        <v>91</v>
+      </c>
       <c r="E2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="J2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" s="30" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{CB4A40A0-7060-4ED2-9352-333B863988E4}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8187711A-441A-49E1-A966-B7B2CA48E69F}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.88671875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="16.88671875" style="1"/>
+    <col min="1" max="7" width="16.88671875" style="1"/>
+    <col min="8" max="8" width="56" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="56" style="1" customWidth="1"/>
+    <col min="10" max="10" width="41.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="16.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1874,43 +2746,68 @@
         <v>10</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="144" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>89</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>19</v>
+        <v>57</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>81</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>20</v>
+        <v>80</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="I2" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" s="31" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{8554854B-D699-4365-89E4-144F052888B8}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
all đồ án 100%
</commit_message>
<xml_diff>
--- a/Đo_An/HoanThanhDangNhap/bin/Debug/Resources/Du lieu cau hoi/thu vien ma loi.xlsx
+++ b/Đo_An/HoanThanhDangNhap/bin/Debug/Resources/Du lieu cau hoi/thu vien ma loi.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Đăng_Quý_UTE_K19\Đo_An\HoanThanhDangNhap\bin\Debug\Resources\Du lieu cau hoi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Đồ án tốt nghiệp\doantn\10-1\Dang_Quy_UTE_k19\Đo_An\HoanThanhDangNhap\bin\Debug\Resources\Du lieu cau hoi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE7D08E-7171-4553-B80A-83C649CF407D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="15" r:id="rId1"/>
@@ -26,6 +25,7 @@
     <sheet name="11" sheetId="3" r:id="rId11"/>
     <sheet name="12" sheetId="4" r:id="rId12"/>
     <sheet name="13" sheetId="5" r:id="rId13"/>
+    <sheet name="14" sheetId="23" r:id="rId14"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="131">
   <si>
     <t>dap an 2</t>
   </si>
@@ -513,11 +513,14 @@
   <si>
     <t>\\Resources\\tong hop final wiring\\40.png</t>
   </si>
+  <si>
+    <t>COMP1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -595,7 +598,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -655,21 +658,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -707,6 +721,15 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1021,23 +1044,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K1" sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="18.77734375" style="5"/>
-    <col min="4" max="4" width="41.33203125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="18.77734375" style="5"/>
-    <col min="6" max="6" width="46.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="194.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="66.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="18.77734375" style="5"/>
+    <col min="1" max="3" width="18.77734375" style="4"/>
+    <col min="4" max="4" width="41.33203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="18.77734375" style="4"/>
+    <col min="6" max="6" width="46.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="70" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="66.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="18.77734375" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
@@ -1050,63 +1073,63 @@
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="101.4" x14ac:dyDescent="0.35">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="K2" s="23" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1120,28 +1143,28 @@
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="11" t="s">
         <v>28</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="25" t="s">
+      <c r="K3" s="23" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1149,206 +1172,206 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="18"/>
+      <c r="D4" s="16"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
     </row>
     <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="18"/>
+      <c r="D5" s="16"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="18"/>
+      <c r="D6" s="16"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="18"/>
+      <c r="D7" s="16"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="18"/>
+      <c r="D8" s="16"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="18"/>
+      <c r="D9" s="16"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="18"/>
+      <c r="D10" s="16"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="18"/>
+      <c r="D11" s="16"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="18"/>
+      <c r="D12" s="16"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="18"/>
+      <c r="D13" s="16"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="18"/>
+      <c r="D14" s="16"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="20"/>
+      <c r="D15" s="18"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
     </row>
     <row r="16" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="20"/>
+      <c r="D16" s="18"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
     </row>
     <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="20"/>
+      <c r="D17" s="18"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
     </row>
     <row r="18" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="18"/>
+      <c r="D18" s="16"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="18"/>
+      <c r="D19" s="16"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="18"/>
+      <c r="D20" s="16"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="18"/>
+      <c r="D21" s="16"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="G2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="G3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="G2" r:id="rId3"/>
+    <hyperlink ref="G3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -1356,20 +1379,20 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView topLeftCell="E3" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="7" width="14.21875" style="5"/>
-    <col min="8" max="8" width="41.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41.5546875" style="5" customWidth="1"/>
-    <col min="10" max="10" width="31.77734375" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="14.21875" style="5"/>
+    <col min="1" max="7" width="14.21875" style="4"/>
+    <col min="8" max="8" width="41.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.5546875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="31.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="14.21875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
@@ -1382,28 +1405,28 @@
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1417,28 +1440,28 @@
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="11" t="s">
         <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="K2" s="23" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1452,28 +1475,28 @@
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="8" t="s">
         <v>86</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="10" t="s">
         <v>104</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="K3" s="25" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1487,39 +1510,39 @@
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="8" t="s">
         <v>83</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="10" t="s">
         <v>104</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K4" s="27" t="s">
+      <c r="K4" s="25" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
-    <hyperlink ref="G2" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
-    <hyperlink ref="F3" r:id="rId3" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
-    <hyperlink ref="F4" r:id="rId4" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
-    <hyperlink ref="G3" r:id="rId5" xr:uid="{00000000-0004-0000-0900-000004000000}"/>
-    <hyperlink ref="G4" r:id="rId6" xr:uid="{00000000-0004-0000-0900-000005000000}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId2"/>
+    <hyperlink ref="F3" r:id="rId3"/>
+    <hyperlink ref="F4" r:id="rId4"/>
+    <hyperlink ref="G3" r:id="rId5"/>
+    <hyperlink ref="G4" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>
@@ -1527,11 +1550,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.6640625" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1556,28 +1579,28 @@
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1591,28 +1614,28 @@
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="8" t="s">
         <v>83</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="20" t="s">
         <v>104</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="27" t="s">
+      <c r="K2" s="25" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1620,66 +1643,66 @@
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="10"/>
+      <c r="D3" s="8"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="22"/>
-      <c r="K3" s="27"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="20"/>
+      <c r="K3" s="25"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="10"/>
+      <c r="D4" s="8"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="22"/>
-      <c r="K4" s="27"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="20"/>
+      <c r="K4" s="25"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
     </row>
     <row r="17" spans="8:9" x14ac:dyDescent="0.35">
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
-    <hyperlink ref="G2" r:id="rId2" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1687,11 +1710,11 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.6640625" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1716,28 +1739,28 @@
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1751,46 +1774,46 @@
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="11" t="s">
         <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="10" t="s">
         <v>104</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="K2" s="27" t="s">
+      <c r="K2" s="25" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
-    <hyperlink ref="G2" r:id="rId2" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1815,28 +1838,28 @@
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1850,93 +1873,154 @@
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="11" t="s">
         <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="10" t="s">
         <v>104</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="K2" s="27" t="s">
+      <c r="K2" s="25" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="90" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="K3" s="27" t="s">
-        <v>57</v>
-      </c>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="D3" s="25"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
-    <hyperlink ref="G2" r:id="rId2" xr:uid="{00000000-0004-0000-0C00-000001000000}"/>
-    <hyperlink ref="F3" r:id="rId3" xr:uid="{00000000-0004-0000-0C00-000002000000}"/>
-    <hyperlink ref="G3" r:id="rId4" xr:uid="{00000000-0004-0000-0C00-000003000000}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="10" max="10" width="83.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="139.19999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" s="25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="16.21875" style="5"/>
-    <col min="4" max="4" width="32.5546875" style="5" customWidth="1"/>
-    <col min="5" max="7" width="16.21875" style="5"/>
-    <col min="8" max="8" width="68.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="68.6640625" style="5" customWidth="1"/>
-    <col min="10" max="16384" width="16.21875" style="5"/>
+    <col min="1" max="3" width="16.21875" style="4"/>
+    <col min="4" max="4" width="32.5546875" style="4" customWidth="1"/>
+    <col min="5" max="7" width="16.21875" style="4"/>
+    <col min="8" max="8" width="68.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="68.6640625" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="16.21875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
@@ -1949,28 +2033,28 @@
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1984,56 +2068,56 @@
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="11" t="s">
         <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="K2" s="23" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="G2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="K1" sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="16.77734375" style="5"/>
-    <col min="4" max="4" width="44.21875" style="5" customWidth="1"/>
-    <col min="5" max="7" width="16.77734375" style="5"/>
-    <col min="8" max="8" width="68.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="68.6640625" style="5" customWidth="1"/>
-    <col min="10" max="16384" width="16.77734375" style="5"/>
+    <col min="1" max="3" width="16.77734375" style="4"/>
+    <col min="4" max="4" width="44.21875" style="4" customWidth="1"/>
+    <col min="5" max="7" width="16.77734375" style="4"/>
+    <col min="8" max="8" width="68.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="68.6640625" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="16.77734375" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
@@ -2046,28 +2130,28 @@
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2081,28 +2165,28 @@
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="11" t="s">
         <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="K2" s="23" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2116,48 +2200,48 @@
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="11" t="s">
         <v>80</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="25" t="s">
+      <c r="K3" s="23" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="G2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="G3" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="G2" r:id="rId3"/>
+    <hyperlink ref="G3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2180,28 +2264,28 @@
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2215,46 +2299,46 @@
       <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="11" t="s">
         <v>81</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="10" t="s">
         <v>94</v>
       </c>
       <c r="J2" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="K2" s="24" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="G2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2277,28 +2361,28 @@
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2310,72 +2394,72 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>81</v>
+        <v>6</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="10" t="s">
         <v>95</v>
       </c>
       <c r="J2" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="K2" s="24" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
+      <c r="A3" s="10"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
+      <c r="A4" s="10"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
+      <c r="A5" s="10"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
+      <c r="A6" s="10"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
+      <c r="A7" s="10"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
+      <c r="A8" s="10"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
+      <c r="A9" s="10"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
+      <c r="A10" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="G2" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2395,28 +2479,28 @@
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2430,28 +2514,28 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="11" t="s">
         <v>82</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="10" t="s">
         <v>98</v>
       </c>
       <c r="J2" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="K2" s="24" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2465,28 +2549,28 @@
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="11" t="s">
         <v>81</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="10" t="s">
         <v>98</v>
       </c>
       <c r="J3" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="26" t="s">
+      <c r="K3" s="24" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2500,50 +2584,50 @@
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="11" t="s">
         <v>28</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="10" t="s">
         <v>98</v>
       </c>
       <c r="J4" t="s">
         <v>56</v>
       </c>
-      <c r="K4" s="26" t="s">
+      <c r="K4" s="24" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
-    <hyperlink ref="G2" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
-    <hyperlink ref="G3" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
-    <hyperlink ref="F4" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
-    <hyperlink ref="G4" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="G2" r:id="rId3"/>
+    <hyperlink ref="G3" r:id="rId4"/>
+    <hyperlink ref="F4" r:id="rId5"/>
+    <hyperlink ref="G4" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="K1" sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2566,28 +2650,28 @@
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2601,46 +2685,46 @@
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="11" t="s">
         <v>81</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="10" t="s">
         <v>98</v>
       </c>
       <c r="J2" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="K2" s="24" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-    <hyperlink ref="G2" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="K1" sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2661,28 +2745,28 @@
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2696,46 +2780,46 @@
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="11" t="s">
         <v>83</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="10" t="s">
         <v>101</v>
       </c>
       <c r="J2" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="K2" s="24" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
-    <hyperlink ref="G2" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.88671875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -2757,70 +2841,70 @@
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="6" t="s">
+      <c r="H1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="144" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="10" t="s">
         <v>101</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="27" t="s">
+      <c r="K2" s="25" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
-    <hyperlink ref="G2" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>